<commit_message>
generated the data as xlsx files insted of csv
</commit_message>
<xml_diff>
--- a/data/philippines/analysis/agusan/flood_trigger_analysis_2025_10_5yr_lead3d.xlsx
+++ b/data/philippines/analysis/agusan/flood_trigger_analysis_2025_10_5yr_lead3d.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA29"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3397,6 +3397,107 @@
       </c>
       <c r="AA29" t="n">
         <v>-76.42992170171001</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>philippines</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Agusan River Basin</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>agusan</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Nia Pumping Station</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>G5368</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>primary</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>3</v>
+      </c>
+      <c r="J30" t="n">
+        <v>8.874999999999865</v>
+      </c>
+      <c r="K30" t="n">
+        <v>125.5749999999995</v>
+      </c>
+      <c r="L30" t="n">
+        <v>5</v>
+      </c>
+      <c r="M30" t="n">
+        <v>4709.973879596918</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>3193.342710267902</v>
+      </c>
+      <c r="P30" t="n">
+        <v>4709.973879596918</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>50</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1034.98828125</v>
+      </c>
+      <c r="U30" t="n">
+        <v>1097.994262695312</v>
+      </c>
+      <c r="V30" t="n">
+        <v>764.4375</v>
+      </c>
+      <c r="W30" t="n">
+        <v>1826.0546875</v>
+      </c>
+      <c r="X30" t="n">
+        <v>920.83203125</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>1198.337890625</v>
+      </c>
+      <c r="Z30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>-78.02560464860635</v>
       </c>
     </row>
   </sheetData>
@@ -3410,7 +3511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA29"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6383,6 +6484,107 @@
         <v>-77.65252691384018</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>philippines</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Agusan River Basin</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>agusan</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Talacogon Municipal Hall</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>G4945</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>secondary</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>3</v>
+      </c>
+      <c r="J30" t="n">
+        <v>8.424999999999859</v>
+      </c>
+      <c r="K30" t="n">
+        <v>125.7749999999995</v>
+      </c>
+      <c r="L30" t="n">
+        <v>5</v>
+      </c>
+      <c r="M30" t="n">
+        <v>3363.250778297076</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>2342.691130371584</v>
+      </c>
+      <c r="P30" t="n">
+        <v>3363.250778297076</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>50</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>684.63671875</v>
+      </c>
+      <c r="U30" t="n">
+        <v>736.4121704101562</v>
+      </c>
+      <c r="V30" t="n">
+        <v>450.953125</v>
+      </c>
+      <c r="W30" t="n">
+        <v>1507.0390625</v>
+      </c>
+      <c r="X30" t="n">
+        <v>581.0234375</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>782.27734375</v>
+      </c>
+      <c r="Z30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>-79.64360186377021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added 3 year RP line in Guetamala hydrographs
</commit_message>
<xml_diff>
--- a/data/philippines/analysis/agusan/flood_trigger_analysis_2025_10_5yr_lead3d.xlsx
+++ b/data/philippines/analysis/agusan/flood_trigger_analysis_2025_10_5yr_lead3d.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3498,6 +3498,208 @@
       </c>
       <c r="AA30" t="n">
         <v>-78.02560464860635</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>philippines</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Agusan River Basin</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>agusan</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Nia Pumping Station</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>G5368</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>primary</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2025-10-30</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>3</v>
+      </c>
+      <c r="J31" t="n">
+        <v>8.874999999999865</v>
+      </c>
+      <c r="K31" t="n">
+        <v>125.5749999999995</v>
+      </c>
+      <c r="L31" t="n">
+        <v>5</v>
+      </c>
+      <c r="M31" t="n">
+        <v>4709.973879596918</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>3193.342710267902</v>
+      </c>
+      <c r="P31" t="n">
+        <v>4709.973879596918</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>50</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>982.4140625</v>
+      </c>
+      <c r="U31" t="n">
+        <v>997.2823486328125</v>
+      </c>
+      <c r="V31" t="n">
+        <v>735.6953125</v>
+      </c>
+      <c r="W31" t="n">
+        <v>1445.9765625</v>
+      </c>
+      <c r="X31" t="n">
+        <v>881.123046875</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>1074.212890625</v>
+      </c>
+      <c r="Z31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>-79.14183629009689</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>philippines</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Agusan River Basin</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>agusan</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Nia Pumping Station</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>G5368</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>primary</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J32" t="n">
+        <v>8.874999999999865</v>
+      </c>
+      <c r="K32" t="n">
+        <v>125.5749999999995</v>
+      </c>
+      <c r="L32" t="n">
+        <v>5</v>
+      </c>
+      <c r="M32" t="n">
+        <v>4709.973879596918</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="O32" t="n">
+        <v>3193.342710267902</v>
+      </c>
+      <c r="P32" t="n">
+        <v>4709.973879596918</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>50</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>869.40234375</v>
+      </c>
+      <c r="U32" t="n">
+        <v>878.986572265625</v>
+      </c>
+      <c r="V32" t="n">
+        <v>734.5859375</v>
+      </c>
+      <c r="W32" t="n">
+        <v>1094.109375</v>
+      </c>
+      <c r="X32" t="n">
+        <v>800.96484375</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>964.27734375</v>
+      </c>
+      <c r="Z32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>-81.54124914543254</v>
       </c>
     </row>
   </sheetData>
@@ -3511,7 +3713,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6585,6 +6787,208 @@
         <v>-79.64360186377021</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>philippines</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Agusan River Basin</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>agusan</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Talacogon Municipal Hall</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>G4945</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>secondary</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2025-10-30</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>3</v>
+      </c>
+      <c r="J31" t="n">
+        <v>8.424999999999859</v>
+      </c>
+      <c r="K31" t="n">
+        <v>125.7749999999995</v>
+      </c>
+      <c r="L31" t="n">
+        <v>5</v>
+      </c>
+      <c r="M31" t="n">
+        <v>3363.250778297076</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>2342.691130371584</v>
+      </c>
+      <c r="P31" t="n">
+        <v>3363.250778297076</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>50</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>676.140625</v>
+      </c>
+      <c r="U31" t="n">
+        <v>680.6256103515625</v>
+      </c>
+      <c r="V31" t="n">
+        <v>488.8515625</v>
+      </c>
+      <c r="W31" t="n">
+        <v>985.921875</v>
+      </c>
+      <c r="X31" t="n">
+        <v>588.794921875</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>745.98828125</v>
+      </c>
+      <c r="Z31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>-79.89621739291317</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>philippines</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Agusan River Basin</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>agusan</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Talacogon Municipal Hall</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>G4945</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>secondary</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J32" t="n">
+        <v>8.424999999999859</v>
+      </c>
+      <c r="K32" t="n">
+        <v>125.7749999999995</v>
+      </c>
+      <c r="L32" t="n">
+        <v>5</v>
+      </c>
+      <c r="M32" t="n">
+        <v>3363.250778297076</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="O32" t="n">
+        <v>2342.691130371584</v>
+      </c>
+      <c r="P32" t="n">
+        <v>3363.250778297076</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>50</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>555.4453125</v>
+      </c>
+      <c r="U32" t="n">
+        <v>570.4659423828125</v>
+      </c>
+      <c r="V32" t="n">
+        <v>459.1796875</v>
+      </c>
+      <c r="W32" t="n">
+        <v>736.265625</v>
+      </c>
+      <c r="X32" t="n">
+        <v>509.15625</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>623.27734375</v>
+      </c>
+      <c r="Z32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>-83.48486779266457</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>